<commit_message>
v2.0.13 - HtmlEorkbookWriter: use relative links if possible
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel/Development/lib/meja/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB7228-2E20-274F-BE4F-698208E126A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30568A89-F03A-014E-A62A-8150C6C7BAB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8660" yWindow="1840" windowWidth="44960" windowHeight="18620" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16660" yWindow="3440" windowWidth="44960" windowHeight="18620" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alignment Test" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="350">
   <si>
     <t>Left</t>
   </si>
@@ -1468,7 +1468,19 @@
     <t>Email Developer</t>
   </si>
   <si>
-    <t>Link to Websites</t>
+    <t>Links to files</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>test.xlsx</t>
+  </si>
+  <si>
+    <t>test.xls</t>
+  </si>
+  <si>
+    <t>Links to Websites</t>
   </si>
 </sst>
 </file>
@@ -5795,6 +5807,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="386" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5804,7 +5817,6 @@
     <xf numFmtId="0" fontId="0" fillId="389" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -9048,10 +9060,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="538" t="s">
+      <c r="A1" s="539" t="s">
         <v>314</v>
       </c>
-      <c r="B1" s="538"/>
+      <c r="B1" s="539"/>
       <c r="C1" s="444" t="s">
         <v>341</v>
       </c>
@@ -9060,11 +9072,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="539" t="s">
+      <c r="A2" s="540" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="539"/>
-      <c r="C2" s="540" t="s">
+      <c r="B2" s="540"/>
+      <c r="C2" s="541" t="s">
         <v>316</v>
       </c>
       <c r="D2" s="444" t="s">
@@ -9072,16 +9084,16 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="539"/>
-      <c r="B3" s="539"/>
-      <c r="C3" s="540"/>
+      <c r="A3" s="540"/>
+      <c r="B3" s="540"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="444" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="539"/>
-      <c r="B4" s="539"/>
+      <c r="A4" s="540"/>
+      <c r="B4" s="540"/>
       <c r="C4" s="444" t="s">
         <v>341</v>
       </c>
@@ -9093,10 +9105,10 @@
       <c r="A5" s="444" t="s">
         <v>341</v>
       </c>
-      <c r="B5" s="538" t="s">
+      <c r="B5" s="539" t="s">
         <v>314</v>
       </c>
-      <c r="C5" s="538"/>
+      <c r="C5" s="539"/>
       <c r="D5" s="444" t="s">
         <v>341</v>
       </c>
@@ -9285,10 +9297,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740A3BD5-63EB-6543-A84C-9EAD8F792455}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9297,26 +9309,43 @@
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="541" t="s">
+      <c r="B1" s="538" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="538" t="s">
+        <v>347</v>
+      </c>
+      <c r="D1" s="538" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B2" s="538" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>343</v>
       </c>
-      <c r="B2" s="541" t="s">
+      <c r="B3" s="538" t="s">
         <v>344</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B7AE0023-61CA-7C48-8A55-16A22EB4C539}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{2827D3D1-7B7E-DE46-AA84-AD96A09CDE9E}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{657FDB47-A01F-1F46-A2B3-CD05320173AD}"/>
+    <hyperlink ref="C1" r:id="rId2" xr:uid="{2D58A05B-5EE8-F640-A0BC-F32D67A83C6A}"/>
+    <hyperlink ref="D1" r:id="rId3" xr:uid="{7D8DD879-ED6E-9C4F-AF78-EBB7D0189BC4}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{DE926EEC-ED32-0843-8687-CB46A2269B1F}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{55C10AD2-B46E-CA4F-BD5F-D0A096314524}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
display links in color defined by cell style
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel/Development/lib/meja/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A92E87-EE9C-BD40-B9B3-E7E570C1E4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9A56CC-C405-0F43-82C5-0D986ABDC94D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="3440" windowWidth="44960" windowHeight="18620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="3440" windowWidth="44960" windowHeight="18620" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alignment Test" sheetId="1" r:id="rId1"/>
@@ -1487,7 +1487,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1730,6 +1730,14 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -4484,7 +4492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="542">
+  <cellXfs count="543">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5817,6 +5825,7 @@
     <xf numFmtId="0" fontId="0" fillId="389" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -6226,7 +6235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9299,8 +9308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740A3BD5-63EB-6543-A84C-9EAD8F792455}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9316,7 +9325,7 @@
       <c r="B1" s="538" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="538" t="s">
+      <c r="C1" s="542" t="s">
         <v>347</v>
       </c>
       <c r="D1" s="538" t="s">

</xml_diff>